<commit_message>
cambio de path, tercera etapa y guardado de respuestas
</commit_message>
<xml_diff>
--- a/files/BernardoRivero.xlsx
+++ b/files/BernardoRivero.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,6 +507,16 @@
           <t>CCEE</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>respuesta</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>razon</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -534,7 +544,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> C',</t>
+          <t xml:space="preserve"> F, C'</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -549,7 +559,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A,</t>
+          <t xml:space="preserve"> A</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -565,6 +575,156 @@
       <c r="L2" t="inlineStr">
         <is>
           <t>?</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>un bicho</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>es gris</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> F, C</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Fi</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>un fuego</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>es rojo</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> F</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> H, Hd</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Po3</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>?</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>personas</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>piernas</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrección de consignas del domain
</commit_message>
<xml_diff>
--- a/files/BernardoRivero.xlsx
+++ b/files/BernardoRivero.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -544,7 +544,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> F, C'</t>
+          <t xml:space="preserve"> F,</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -559,12 +559,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> A</t>
+          <t xml:space="preserve"> Xy,</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Po1</t>
+          <t>?</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -579,152 +579,12 @@
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>un bicho</t>
+          <t>una radiografia</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>es gris</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> F, C</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Fi</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>fuego</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>es rojo</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> F</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> H, Hd</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Po3</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>?</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>persona</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>pierna</t>
+          <t>?</t>
         </is>
       </c>
     </row>

</xml_diff>